<commit_message>
Updated the model for publication
</commit_message>
<xml_diff>
--- a/Data/Metadata.xlsx
+++ b/Data/Metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luxma\OneDrive\Documents\GitHub\OREI_Multimodel-inference\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luxma\OneDrive\Documents\GitHub\OREI_ML_Inference\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B86B0A6-AAE7-4871-8AFF-F1B3D4C4C79E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA3363B8-BE03-4B3F-B5B4-9A387F5FC19D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17535" yWindow="1890" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -754,8 +754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:XFD67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>